<commit_message>
changes in css and uploaded sample file
</commit_message>
<xml_diff>
--- a/sample/upload.xlsx
+++ b/sample/upload.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Course</t>
   </si>
@@ -34,10 +34,43 @@
     <t>Minimum Students</t>
   </si>
   <si>
-    <t>Credits</t>
-  </si>
-  <si>
     <t>Subject Costs</t>
+  </si>
+  <si>
+    <t>TERCER CUATRIMESTRE</t>
+  </si>
+  <si>
+    <t>PRIMER CUATRIMESTRE,SEGUNDO CUATRIMESTRE</t>
+  </si>
+  <si>
+    <t>2015-02</t>
+  </si>
+  <si>
+    <t>Course Code</t>
+  </si>
+  <si>
+    <t>CON-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.CONTABILIDAD COMPUTARIZADA </t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>2015 - 02 N</t>
+  </si>
+  <si>
+    <t>1.REFRIGERACION INDUSTRIAL</t>
+  </si>
+  <si>
+    <t>REF-01</t>
+  </si>
+  <si>
+    <t>SISTEMA DE EMPRESAS</t>
+  </si>
+  <si>
+    <t>MEDIO AMBIENTE,NEUMÃTICA</t>
   </si>
 </sst>
 </file>
@@ -126,7 +159,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -136,9 +169,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -441,47 +471,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.5">
+    <row r="1" spans="1:9" ht="31.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="G2" s="3">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>500</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3" s="3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>100</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in import csv functionality
</commit_message>
<xml_diff>
--- a/sample/upload.xlsx
+++ b/sample/upload.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Course</t>
   </si>
@@ -37,40 +37,16 @@
     <t>Subject Costs</t>
   </si>
   <si>
-    <t>TERCER CUATRIMESTRE</t>
-  </si>
-  <si>
-    <t>PRIMER CUATRIMESTRE,SEGUNDO CUATRIMESTRE</t>
-  </si>
-  <si>
-    <t>2015-02</t>
-  </si>
-  <si>
     <t>Course Code</t>
   </si>
   <si>
-    <t>CON-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.CONTABILIDAD COMPUTARIZADA </t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
-    <t>2015 - 02 N</t>
-  </si>
-  <si>
-    <t>1.REFRIGERACION INDUSTRIAL</t>
-  </si>
-  <si>
-    <t>REF-01</t>
-  </si>
-  <si>
-    <t>SISTEMA DE EMPRESAS</t>
-  </si>
-  <si>
-    <t>MEDIO AMBIENTE,NEUMÃTICA</t>
+    <t>Subject Code</t>
+  </si>
+  <si>
+    <t>Subject PRE-Requistie Code</t>
   </si>
 </sst>
 </file>
@@ -471,28 +447,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="44.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" style="3" customWidth="1"/>
+    <col min="4" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5">
+    <row r="1" spans="1:11" ht="31.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -500,78 +476,26 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="F2">
-        <v>100</v>
-      </c>
-      <c r="G2" s="3">
-        <v>10</v>
-      </c>
-      <c r="H2">
-        <v>500</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3">
-        <v>20</v>
-      </c>
-      <c r="G3" s="3">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <v>100</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>